<commit_message>
EPBDS-10341 EPBDS-9590 EPBDS-8844 Fix compilation when custom.spreadsheet.type=false
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10341_SpreadsheetResult_class.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-10341_SpreadsheetResult_class.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A00F161-3FCD-49AE-824C-EF4876160117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F28BA3-8335-46B5-9D3F-13F73962A423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31740" yWindow="2940" windowWidth="21600" windowHeight="11385" xr2:uid="{E59F7472-A9D2-4FC2-8ED3-4C22BD94DB84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E59F7472-A9D2-4FC2-8ED3-4C22BD94DB84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
-  <si>
-    <t>Spreadsheet SpreadsheetResult SRClass(SpreadsheetResult sr, String s)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Step</t>
   </si>
@@ -47,39 +44,21 @@
     <t>case1</t>
   </si>
   <si>
-    <t>=sr.class</t>
-  </si>
-  <si>
     <t>case2</t>
   </si>
   <si>
     <t>case3</t>
   </si>
   <si>
-    <t>=String.class</t>
-  </si>
-  <si>
     <t>case4</t>
   </si>
   <si>
-    <t>= s.class</t>
-  </si>
-  <si>
-    <t>=SpreadsheetResult.class</t>
-  </si>
-  <si>
     <t>sr</t>
   </si>
   <si>
     <t>Sr</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>_res_.$Value$case1</t>
   </si>
   <si>
@@ -92,15 +71,9 @@
     <t>_res_.$Value$case4</t>
   </si>
   <si>
-    <t>java.lang.String</t>
-  </si>
-  <si>
     <t>org.openl.rules.calc.SpreadsheetResult</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>Test SRClass</t>
   </si>
   <si>
@@ -110,10 +83,97 @@
     <t>SR2</t>
   </si>
   <si>
-    <t>STR1</t>
-  </si>
-  <si>
-    <t>STR2</t>
+    <t>case5</t>
+  </si>
+  <si>
+    <t>_res_.$Value$case5</t>
+  </si>
+  <si>
+    <t>case6</t>
+  </si>
+  <si>
+    <t>_res_.$Value$case6</t>
+  </si>
+  <si>
+    <t>= org.openl.rules.calc.SpreadsheetResult.class</t>
+  </si>
+  <si>
+    <t>= sr.class</t>
+  </si>
+  <si>
+    <t>= SpreadsheetResult.class</t>
+  </si>
+  <si>
+    <t>case7</t>
+  </si>
+  <si>
+    <t>case8</t>
+  </si>
+  <si>
+    <t>_res_.$Value$case7</t>
+  </si>
+  <si>
+    <t>_res_.$Value$case8</t>
+  </si>
+  <si>
+    <t>SR3</t>
+  </si>
+  <si>
+    <t>SR4</t>
+  </si>
+  <si>
+    <t>SR5</t>
+  </si>
+  <si>
+    <t>= SpreadsheetResult.class.getName()</t>
+  </si>
+  <si>
+    <t>= org.openl.rules.calc.SpreadsheetResult.class.getName()</t>
+  </si>
+  <si>
+    <t>_res_.$Value$case9</t>
+  </si>
+  <si>
+    <t>_res_.$Value$case10</t>
+  </si>
+  <si>
+    <t>case9</t>
+  </si>
+  <si>
+    <t>case10</t>
+  </si>
+  <si>
+    <t>SR6</t>
+  </si>
+  <si>
+    <t>SR7</t>
+  </si>
+  <si>
+    <t>SR8</t>
+  </si>
+  <si>
+    <t>= org.openl.rules.calc.SpreadsheetResult.class.name</t>
+  </si>
+  <si>
+    <t>= SpreadsheetResult.class.name</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult SRClass(SpreadsheetResult sr)</t>
+  </si>
+  <si>
+    <t>SR9</t>
+  </si>
+  <si>
+    <t>SR10</t>
+  </si>
+  <si>
+    <t>= toString(org.openl.rules.calc.SpreadsheetResult.class)</t>
+  </si>
+  <si>
+    <t>= toString(SpreadsheetResult.class)</t>
+  </si>
+  <si>
+    <t>class org.openl.rules.calc.SpreadsheetResult</t>
   </si>
 </sst>
 </file>
@@ -185,10 +245,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -506,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DCC082-B645-4260-A0B9-5F0428966443}">
-  <dimension ref="B3:H9"/>
+  <dimension ref="B4:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,133 +583,209 @@
     <col min="4" max="4" width="22.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E3" s="5" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="E4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="E4" s="3" t="s">
+      <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3" t="s">
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>19</v>
+      <c r="F13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:G4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>